<commit_message>
the complete prototype of the project
</commit_message>
<xml_diff>
--- a/src/excel/assigneng.xlsx
+++ b/src/excel/assigneng.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="36">
   <si>
     <t>AssignId</t>
   </si>
@@ -39,51 +39,39 @@
     <t>Assigner</t>
   </si>
   <si>
-    <t>assigneng1</t>
+    <t>assigneng2</t>
+  </si>
+  <si>
+    <t>dhanasekar1</t>
+  </si>
+  <si>
+    <t>shell</t>
+  </si>
+  <si>
+    <t>Once a week</t>
+  </si>
+  <si>
+    <t>Project</t>
   </si>
   <si>
     <t>dhanasekar</t>
   </si>
   <si>
-    <t>ford</t>
-  </si>
-  <si>
-    <t>Once a day</t>
-  </si>
-  <si>
-    <t>trading</t>
+    <t>assigneng3</t>
+  </si>
+  <si>
+    <t>dans1</t>
+  </si>
+  <si>
+    <t>shell india wheels</t>
+  </si>
+  <si>
+    <t>Trading</t>
   </si>
   <si>
     <t>ds</t>
   </si>
   <si>
-    <t>assigneng2</t>
-  </si>
-  <si>
-    <t>dhanasekar1</t>
-  </si>
-  <si>
-    <t>shell</t>
-  </si>
-  <si>
-    <t>Once a week</t>
-  </si>
-  <si>
-    <t>Project</t>
-  </si>
-  <si>
-    <t>assigneng3</t>
-  </si>
-  <si>
-    <t>dans1</t>
-  </si>
-  <si>
-    <t>shell india wheels</t>
-  </si>
-  <si>
-    <t>Trading</t>
-  </si>
-  <si>
     <t>assigneng4</t>
   </si>
   <si>
@@ -93,103 +81,49 @@
     <t>once a week</t>
   </si>
   <si>
-    <t>assigneng5</t>
+    <t>assigneng6</t>
+  </si>
+  <si>
+    <t>dhana</t>
   </si>
   <si>
     <t>sekar</t>
   </si>
   <si>
-    <t>dhana</t>
-  </si>
-  <si>
-    <t>2018-05-04</t>
-  </si>
-  <si>
-    <t>Twice a Day</t>
-  </si>
-  <si>
-    <t>P</t>
-  </si>
-  <si>
-    <t>assigneng6</t>
-  </si>
-  <si>
-    <t>2018-05-01</t>
+    <t>2018-05-13</t>
+  </si>
+  <si>
+    <t>Once a Day</t>
+  </si>
+  <si>
+    <t>kkkkkkk</t>
+  </si>
+  <si>
+    <t>2018-05-06</t>
+  </si>
+  <si>
+    <t>wine</t>
   </si>
   <si>
     <t>assigneng7</t>
   </si>
   <si>
-    <t>2018-05-10</t>
-  </si>
-  <si>
-    <t>Twice a Week</t>
-  </si>
-  <si>
-    <t>S</t>
+    <t>kkkkkkkkk</t>
+  </si>
+  <si>
+    <t>2018-05-12</t>
+  </si>
+  <si>
+    <t>Once a Week</t>
   </si>
   <si>
     <t>assigneng8</t>
   </si>
   <si>
-    <t>2018-05-26</t>
-  </si>
-  <si>
-    <t>Once a Week</t>
-  </si>
-  <si>
-    <t>assigneng9</t>
-  </si>
-  <si>
-    <t>2018-05-27</t>
-  </si>
-  <si>
-    <t>Once a Day</t>
-  </si>
-  <si>
-    <t>assigneng10</t>
-  </si>
-  <si>
-    <t>2018-05-18</t>
+    <t>2018-05-22</t>
   </si>
   <si>
     <t>Tender</t>
-  </si>
-  <si>
-    <t>assigneng11</t>
-  </si>
-  <si>
-    <t>2018-05-12</t>
-  </si>
-  <si>
-    <t>assigneng12</t>
-  </si>
-  <si>
-    <t>summa</t>
-  </si>
-  <si>
-    <t>2018-05-20</t>
-  </si>
-  <si>
-    <t>assigneng13</t>
-  </si>
-  <si>
-    <t>2018-05-11</t>
-  </si>
-  <si>
-    <t>assigneng14</t>
-  </si>
-  <si>
-    <t>2018-05-13</t>
-  </si>
-  <si>
-    <t>assigneng15</t>
-  </si>
-  <si>
-    <t>2018-05-19</t>
-  </si>
-  <si>
-    <t>assigneng16</t>
   </si>
 </sst>
 </file>
@@ -530,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0"/>
@@ -606,13 +540,13 @@
         <v>25569.00002321759</v>
       </c>
       <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>17</v>
-      </c>
-      <c r="G3" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -620,91 +554,91 @@
         <v>18</v>
       </c>
       <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
         <v>19</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" s="1">
+        <v>43132</v>
+      </c>
+      <c r="E4" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="1">
-        <v>25569.00002321759</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
-      </c>
       <c r="F4" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="G4" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
         <v>22</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
       </c>
       <c r="C5" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="1">
-        <v>43132</v>
+      <c r="D5" t="s">
+        <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F5" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="G5" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" t="s">
         <v>25</v>
       </c>
-      <c r="B6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" t="s">
         <v>28</v>
-      </c>
-      <c r="E6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" t="s">
-        <v>30</v>
-      </c>
-      <c r="G6" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" t="s">
         <v>31</v>
       </c>
-      <c r="B7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>32</v>
       </c>
-      <c r="E7" t="s">
-        <v>29</v>
-      </c>
       <c r="F7" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="G7" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -712,229 +646,22 @@
         <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="D8" t="s">
         <v>34</v>
       </c>
       <c r="E8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" t="s">
         <v>35</v>
       </c>
-      <c r="F8" t="s">
-        <v>36</v>
-      </c>
       <c r="G8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" t="s">
-        <v>39</v>
-      </c>
-      <c r="F9" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" t="s">
-        <v>42</v>
-      </c>
-      <c r="F10" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>43</v>
-      </c>
-      <c r="B11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" t="s">
-        <v>44</v>
-      </c>
-      <c r="E11" t="s">
-        <v>42</v>
-      </c>
-      <c r="F11" t="s">
-        <v>45</v>
-      </c>
-      <c r="G11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>46</v>
-      </c>
-      <c r="B12" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" t="s">
-        <v>47</v>
-      </c>
-      <c r="E12" t="s">
-        <v>29</v>
-      </c>
-      <c r="F12" t="s">
-        <v>17</v>
-      </c>
-      <c r="G12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>48</v>
-      </c>
-      <c r="B13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" t="s">
-        <v>49</v>
-      </c>
-      <c r="D13" t="s">
-        <v>50</v>
-      </c>
-      <c r="E13" t="s">
-        <v>39</v>
-      </c>
-      <c r="F13" t="s">
-        <v>45</v>
-      </c>
-      <c r="G13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>51</v>
-      </c>
-      <c r="B14" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" t="s">
-        <v>52</v>
-      </c>
-      <c r="E14" t="s">
-        <v>39</v>
-      </c>
-      <c r="F14" t="s">
-        <v>45</v>
-      </c>
-      <c r="G14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>53</v>
-      </c>
-      <c r="B15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" t="s">
-        <v>54</v>
-      </c>
-      <c r="E15" t="s">
-        <v>42</v>
-      </c>
-      <c r="F15" t="s">
-        <v>45</v>
-      </c>
-      <c r="G15" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>55</v>
-      </c>
-      <c r="B16" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" t="s">
-        <v>56</v>
-      </c>
-      <c r="E16" t="s">
-        <v>42</v>
-      </c>
-      <c r="F16" t="s">
-        <v>45</v>
-      </c>
-      <c r="G16" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>57</v>
-      </c>
-      <c r="B17" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" t="s">
-        <v>34</v>
-      </c>
-      <c r="E17" t="s">
-        <v>29</v>
-      </c>
-      <c r="F17" t="s">
-        <v>17</v>
-      </c>
-      <c r="G17" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified and updated the insertexcel and form2
</commit_message>
<xml_diff>
--- a/src/excel/assigneng.xlsx
+++ b/src/excel/assigneng.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>AssignId</t>
   </si>
@@ -42,82 +42,22 @@
     <t>assigneng2</t>
   </si>
   <si>
-    <t>dhanasekar1</t>
-  </si>
-  <si>
-    <t>shell</t>
-  </si>
-  <si>
-    <t>Once a week</t>
-  </si>
-  <si>
-    <t>Project</t>
-  </si>
-  <si>
-    <t>dhanasekar</t>
-  </si>
-  <si>
-    <t>assigneng3</t>
-  </si>
-  <si>
-    <t>dans1</t>
-  </si>
-  <si>
-    <t>shell india wheels</t>
-  </si>
-  <si>
-    <t>Trading</t>
+    <t>sekar</t>
+  </si>
+  <si>
+    <t>jjjjjj</t>
+  </si>
+  <si>
+    <t>2018-05-12</t>
+  </si>
+  <si>
+    <t>Once a Day</t>
+  </si>
+  <si>
+    <t>Tender</t>
   </si>
   <si>
     <t>ds</t>
-  </si>
-  <si>
-    <t>assigneng4</t>
-  </si>
-  <si>
-    <t>wheels india</t>
-  </si>
-  <si>
-    <t>once a week</t>
-  </si>
-  <si>
-    <t>assigneng6</t>
-  </si>
-  <si>
-    <t>dhana</t>
-  </si>
-  <si>
-    <t>sekar</t>
-  </si>
-  <si>
-    <t>2018-05-13</t>
-  </si>
-  <si>
-    <t>Once a Day</t>
-  </si>
-  <si>
-    <t>kkkkkkk</t>
-  </si>
-  <si>
-    <t>2018-05-06</t>
-  </si>
-  <si>
-    <t>wine</t>
-  </si>
-  <si>
-    <t>assigneng8</t>
-  </si>
-  <si>
-    <t>2018-05-18</t>
-  </si>
-  <si>
-    <t>Once a Week</t>
-  </si>
-  <si>
-    <t>typical solution</t>
-  </si>
-  <si>
-    <t>2018-05-12</t>
   </si>
 </sst>
 </file>
@@ -153,9 +93,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -458,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0"/>
@@ -507,155 +446,17 @@
       <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="1">
-        <v>25569.00002321759</v>
+      <c r="D2" t="s">
+        <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
         <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="1">
-        <v>25569.00002321759</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="1">
-        <v>43132</v>
-      </c>
-      <c r="E4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>